<commit_message>
Add existing project files
</commit_message>
<xml_diff>
--- a/Stocks_top_Perf.xlsx
+++ b/Stocks_top_Perf.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\genAI\project_Stock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F940564-40EB-4770-B57F-FC10D888A604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5740F266-525B-4C5D-BDEE-5748833A66DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-114" yWindow="-114" windowWidth="19704" windowHeight="10579" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$1206</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -6222,8 +6225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{863BA4EA-B06C-476F-99E0-925C8BCD751A}">
   <dimension ref="A1:L1206"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -49667,6 +49670,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L1206" xr:uid="{863BA4EA-B06C-476F-99E0-925C8BCD751A}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>